<commit_message>
3 largest numbers added
</commit_message>
<xml_diff>
--- a/Algorithms_solved.xlsx
+++ b/Algorithms_solved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shehryarbajwa/algorithms-challenges/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C94B98-1EF9-994C-A689-60966A204852}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630DBE24-85E7-EA43-807A-760ADA715C2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="60" windowWidth="28040" windowHeight="15900" xr2:uid="{5B13E3C5-C034-6249-A945-F210C27A470A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
   <si>
     <t>Problem</t>
   </si>
@@ -121,6 +121,33 @@
   </si>
   <si>
     <t>Recursively, Memoization, Iteratively</t>
+  </si>
+  <si>
+    <t>Product Sum</t>
+  </si>
+  <si>
+    <t>Recursion, Multiplier</t>
+  </si>
+  <si>
+    <t>If a Special Array contains other special arrays, it can be solved recursively</t>
+  </si>
+  <si>
+    <t>How is the multiplier calculated?</t>
+  </si>
+  <si>
+    <t>Setting pointers</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Recursion</t>
+  </si>
+  <si>
+    <t>Binary search is sorted</t>
+  </si>
+  <si>
+    <t>Is the list sorted?</t>
   </si>
 </sst>
 </file>
@@ -486,23 +513,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692D23BF-E5BD-4744-931C-2F3DDC23964E}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
-    <col min="2" max="2" width="28.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="22.1640625" customWidth="1"/>
     <col min="5" max="5" width="22.5" customWidth="1"/>
     <col min="6" max="6" width="21.83203125" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" customWidth="1"/>
     <col min="8" max="8" width="31.33203125" customWidth="1"/>
-    <col min="9" max="9" width="70.6640625" customWidth="1"/>
+    <col min="9" max="9" width="71.6640625" customWidth="1"/>
     <col min="10" max="10" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -668,7 +695,9 @@
       <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="3">
         <v>43952</v>
@@ -708,6 +737,66 @@
         <v>31</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3">
+        <v>43983</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="3">
+        <v>43983</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>